<commit_message>
fix: nombre cabecera reporte servicio
</commit_message>
<xml_diff>
--- a/boot/src/main/resources/xlsx/mantenimientosgenerales/servicio.xlsx
+++ b/boot/src/main/resources/xlsx/mantenimientosgenerales/servicio.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14490" windowHeight="2910"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -60,17 +61,17 @@
     <t>${item.idMembresia} - ${item.descripcionMembresia}</t>
   </si>
   <si>
-    <t>Código Servicio</t>
+    <t>${item.idServicio} - ${item.descripcionServicio}</t>
   </si>
   <si>
-    <t>${item.idServicio} - ${item.descripcionServicio}</t>
+    <t>Servicio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +139,14 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -344,6 +353,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -680,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,9 +802,9 @@
         <v>6</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="33"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
@@ -844,7 +856,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="18"/>
@@ -963,6 +975,6 @@
     <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>